<commit_message>
book and media report content update Tue 12/31/2024
</commit_message>
<xml_diff>
--- a/report/books/years/img/Book Data.xlsx
+++ b/report/books/years/img/Book Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Coding\GitHub\venomousprimate.github.io\report\books\years\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C4C52B-D18B-492F-8EA7-EED8212FF0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0CEEB0-F550-43A9-9619-F6ECE7A8B8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="1180" windowWidth="36170" windowHeight="19120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>33</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -648,7 +648,7 @@
                   <c:v>663</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>404</c:v>
+                  <c:v>632</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1813,7 +1813,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1972,10 +1972,10 @@
         <v>2024</v>
       </c>
       <c r="B13" s="1">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C13" s="2">
-        <v>404</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>
@@ -1991,7 +1991,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG46" sqref="AG46"/>
+      <selection activeCell="T56" sqref="T56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
book and media report content update Thu 12/04/2025
</commit_message>
<xml_diff>
--- a/report/books/years/img/Book Data.xlsx
+++ b/report/books/years/img/Book Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Coding\GitHub\venomousprimate.github.io\report\books\years\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0CEEB0-F550-43A9-9619-F6ECE7A8B8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82528335-6E15-4FFD-9E88-0DC996700D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -420,10 +420,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$13</c:f>
+              <c:f>Data!$A$2:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -459,16 +459,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$13</c:f>
+              <c:f>Data!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
@@ -504,6 +507,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -565,10 +571,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$13</c:f>
+              <c:f>Data!$A$2:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
                 </c:pt>
@@ -604,16 +610,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$13</c:f>
+              <c:f>Data!$C$2:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>437</c:v>
                 </c:pt>
@@ -649,6 +658,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>632</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1536,8 +1548,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E59ECF05-A303-4E61-94E1-80E277BB7E68}" name="Table2" displayName="Table2" ref="A1:C13" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:C13" xr:uid="{E59ECF05-A303-4E61-94E1-80E277BB7E68}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E59ECF05-A303-4E61-94E1-80E277BB7E68}" name="Table2" displayName="Table2" ref="A1:C14" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:C14" xr:uid="{E59ECF05-A303-4E61-94E1-80E277BB7E68}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{21C3038C-39C6-48F3-8D5E-1DCADB58F512}" name="Year" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{53538222-D103-4FDA-9681-515D21CBCEA4}" name="Book Count" dataDxfId="1"/>
@@ -1810,10 +1822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1976,6 +1988,17 @@
       </c>
       <c r="C13" s="2">
         <v>632</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>2025</v>
+      </c>
+      <c r="B14" s="1">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2">
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
book and media report content update Mon 12/15/2025
</commit_message>
<xml_diff>
--- a/report/books/years/img/Book Data.xlsx
+++ b/report/books/years/img/Book Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Coding\GitHub\venomousprimate.github.io\report\books\years\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82528335-6E15-4FFD-9E88-0DC996700D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E1F99E-6DB8-444F-9BB7-066EE790BC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,7 +509,7 @@
                   <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1825,7 +1825,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1995,7 +1995,7 @@
         <v>2025</v>
       </c>
       <c r="B14" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2">
         <v>386</v>

</xml_diff>

<commit_message>
book and media report content update Thu 12/18/2025
</commit_message>
<xml_diff>
--- a/report/books/years/img/Book Data.xlsx
+++ b/report/books/years/img/Book Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Coding\GitHub\venomousprimate.github.io\report\books\years\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E1F99E-6DB8-444F-9BB7-066EE790BC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1660755D-DC2D-4C38-9EEA-F78B33A25550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -660,7 +660,7 @@
                   <c:v>632</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>386</c:v>
+                  <c:v>410</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1825,7 +1825,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1998,7 +1998,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="2">
-        <v>386</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>